<commit_message>
Still building rounds. Added utility db files for access.
</commit_message>
<xml_diff>
--- a/pinederby.xlsx
+++ b/pinederby.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Id</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>S3</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>entry</t>
   </si>
 </sst>
 </file>
@@ -5004,9 +5017,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>IF((B2+C2)&lt;=MAX(A2,A17),(B2+C2),(B2+C2-MAX(A2,A17)))</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>